<commit_message>
Second commit after changes
</commit_message>
<xml_diff>
--- a/Dynamic-Financial-Forecast-Model.xlsx
+++ b/Dynamic-Financial-Forecast-Model.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\This PC\Projects\Finance &amp; Business Analyst Related Projects\Dynamic Financial Forcast Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C06663-CD97-4C03-BF48-E994382B4BFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAB498A-AF30-4554-BFF5-045893E6C83C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{51C94CC5-0C2F-6D4D-9C41-E0029B3FD163}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12084" windowHeight="8532" xr2:uid="{51C94CC5-0C2F-6D4D-9C41-E0029B3FD163}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cover Page" sheetId="2" r:id="rId1"/>
-    <sheet name="Forecasting Model" sheetId="1" r:id="rId2"/>
+    <sheet name="Forecasting Model" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
   <si>
     <t>Income Statement</t>
   </si>
@@ -125,62 +124,6 @@
   </si>
   <si>
     <t>Order Fulfillment</t>
-  </si>
-  <si>
-    <r>
-      <t>Get 10%</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> OFF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> our course using coupon code </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EMAIL10</t>
-    </r>
-  </si>
-  <si>
-    <t>Made by Kenji Explains / Career Principles</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>All content is copyright material of Kenji Explains / Career Principles</t>
-  </si>
-  <si>
-    <t>This Excel model may not be reproduced or distributed by any means, including printing, 
-screencapturing, or any other method without the prior permission of the publisher.</t>
-  </si>
-  <si>
-    <t>Get Our Complete Finance &amp; Valuation Course</t>
-  </si>
-  <si>
-    <t>Financial Model Start File</t>
   </si>
   <si>
     <t>Upper Case (Scenario 1)</t>
@@ -204,7 +147,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -293,69 +236,14 @@
     </font>
     <font>
       <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="42"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="50"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="20"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="14"/>
-      <color rgb="FF0432FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,18 +288,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -439,112 +321,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -614,59 +400,19 @@
     <xf numFmtId="17" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="5" xr:uid="{5F59BA89-7615-4281-8BEF-2784D80BF483}"/>
-    <cellStyle name="Hyperlink 2 2" xfId="6" xr:uid="{E46816E3-91A1-429A-9F57-9AA0637835E3}"/>
+    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{5F59BA89-7615-4281-8BEF-2784D80BF483}"/>
+    <cellStyle name="Hyperlink 2 2" xfId="5" xr:uid="{E46816E3-91A1-429A-9F57-9AA0637835E3}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{E91F33F0-9EC6-4D88-A40D-712287F90237}"/>
+    <cellStyle name="Normal 2 2" xfId="3" xr:uid="{E91F33F0-9EC6-4D88-A40D-712287F90237}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -689,50 +435,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2434775</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>190501</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3050985" cy="865353"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27B43E1E-B6CF-49AB-9A62-E8209207EEC6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3717475" y="1428751"/>
-          <a:ext cx="3050985" cy="865353"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1031,129 +733,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625B5DD8-9B40-4EC2-9E5C-82832308D8C6}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="B4:D19"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.5" style="40"/>
-    <col min="2" max="2" width="7.296875" style="40" customWidth="1"/>
-    <col min="3" max="3" width="96.69921875" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.19921875" style="40" customWidth="1"/>
-    <col min="5" max="16384" width="9.5" style="40"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:4" ht="54" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="39"/>
-    </row>
-    <row r="5" spans="2:4" ht="63.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="43"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="41"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="43"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="41"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="43"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="41"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="43"/>
-    </row>
-    <row r="9" spans="2:4" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="B9" s="45"/>
-      <c r="C9" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="47"/>
-    </row>
-    <row r="10" spans="2:4" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="B10" s="45"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="47"/>
-    </row>
-    <row r="11" spans="2:4" s="52" customFormat="1" ht="23.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="50"/>
-      <c r="C11" s="59" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="51"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="41"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="43"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="41"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="43"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="41"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="43"/>
-    </row>
-    <row r="15" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B15" s="41"/>
-      <c r="C15" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="43"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="41"/>
-      <c r="C16" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="43"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="41"/>
-      <c r="C17" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="43"/>
-    </row>
-    <row r="18" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="41"/>
-      <c r="C18" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="43"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="56"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="58"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{7AB64434-E6B6-4877-90B0-C2834D57318A}"/>
-    <hyperlink ref="C15" r:id="rId2" display="Made by Kenji Explains" xr:uid="{386A39F8-F42A-4D89-8B86-9265C130E89F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BAF0A7-6C3E-5B41-B94B-78E46A3C64F1}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:J80"/>
@@ -1227,10 +806,10 @@
       <c r="F4" s="31"/>
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
-      <c r="I4" s="61" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="60">
+      <c r="I4" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="37">
         <v>2</v>
       </c>
     </row>
@@ -1689,7 +1268,7 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="6"/>
@@ -1982,7 +1561,7 @@
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="6"/>
@@ -2274,7 +1853,7 @@
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B64" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="6"/>

</xml_diff>